<commit_message>
Added short file name translations to the tool Basically all translations are now part of the tool
</commit_message>
<xml_diff>
--- a/Lang_files_bat.xlsx
+++ b/Lang_files_bat.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sources\reactos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1E16C61-ABD0-4B52-B233-D7E13403ECE3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AED7C09A-990D-4899-9D7D-C4A36B9FA647}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{3A083AA0-6BDF-4150-85AD-84676BBB71DE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" activeTab="2" xr2:uid="{3A083AA0-6BDF-4150-85AD-84676BBB71DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1853" uniqueCount="1395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="1464">
   <si>
     <t>cacls</t>
   </si>
@@ -5430,6 +5431,213 @@
   <si>
     <t xml:space="preserve">
 </t>
+  </si>
+  <si>
+    <t>C:\sources\reactos\base\applications\winhlp32</t>
+  </si>
+  <si>
+    <t>rsrc.rc</t>
+  </si>
+  <si>
+    <t>En.rc</t>
+  </si>
+  <si>
+    <t>usetup.rc</t>
+  </si>
+  <si>
+    <t>en-US.h</t>
+  </si>
+  <si>
+    <t>avifile_En.rc</t>
+  </si>
+  <si>
+    <t>comctl_En.rc</t>
+  </si>
+  <si>
+    <t>cdlg_En.rc</t>
+  </si>
+  <si>
+    <t>credui.rc</t>
+  </si>
+  <si>
+    <t>credui_En.rc</t>
+  </si>
+  <si>
+    <t>crypt32.rc</t>
+  </si>
+  <si>
+    <t>crypt32_En.rc</t>
+  </si>
+  <si>
+    <t>cryptdlg.rc</t>
+  </si>
+  <si>
+    <t>cryptdlg_En.rc</t>
+  </si>
+  <si>
+    <t>cryptui.rc</t>
+  </si>
+  <si>
+    <t>cryptui_En.rc</t>
+  </si>
+  <si>
+    <t>hhctrl.rc</t>
+  </si>
+  <si>
+    <t>iccvid_En.rc</t>
+  </si>
+  <si>
+    <t>jscript_En.rc</t>
+  </si>
+  <si>
+    <t>version.rc</t>
+  </si>
+  <si>
+    <t>mpr_En.rc</t>
+  </si>
+  <si>
+    <t>msacm.rc</t>
+  </si>
+  <si>
+    <t>msacm_En.rc</t>
+  </si>
+  <si>
+    <t>msi.rc</t>
+  </si>
+  <si>
+    <t>msi_En.rc</t>
+  </si>
+  <si>
+    <t>msrle_En.rc</t>
+  </si>
+  <si>
+    <t>msvfw32_En.rc</t>
+  </si>
+  <si>
+    <t>msvidc32_En.rc</t>
+  </si>
+  <si>
+    <t>oleacc.rc</t>
+  </si>
+  <si>
+    <t>oleacc_En.rc</t>
+  </si>
+  <si>
+    <t>oleaut32.rc</t>
+  </si>
+  <si>
+    <t>oleaut32_En.rc</t>
+  </si>
+  <si>
+    <t>oledlg_En.rc</t>
+  </si>
+  <si>
+    <t>shlwapi_En.rc</t>
+  </si>
+  <si>
+    <t>wininet_En.rc</t>
+  </si>
+  <si>
+    <t>winmm_res.rc</t>
+  </si>
+  <si>
+    <t>winmm_En.rc</t>
+  </si>
+  <si>
+    <t>wldap32.rc</t>
+  </si>
+  <si>
+    <t>wldap32_En.rc</t>
+  </si>
+  <si>
+    <t>localui.rc</t>
+  </si>
+  <si>
+    <t>ui_En.rc</t>
+  </si>
+  <si>
+    <t>cd C:\sources\reactos\base\applications\winhlp32</t>
+  </si>
+  <si>
+    <t>call :lang_add rsrc.rc En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add usetup.rc en-US.h</t>
+  </si>
+  <si>
+    <t>call :lang_add rsrc.rc avifile_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add rsrc.rc comctl_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add rsrc.rc cdlg_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add credui.rc credui_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add crypt32.rc crypt32_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add cryptdlg.rc cryptdlg_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add cryptui.rc cryptui_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add hhctrl.rc En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add rsrc.rc iccvid_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add rsrc.rc jscript_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add version.rc En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add version.rc mpr_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add msacm.rc msacm_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add msi.rc msi_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add rsrc.rc msrle_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add rsrc.rc msvfw32_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add rsrc.rc msvidc32_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add oleacc.rc oleacc_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add oleaut32.rc oleaut32_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add rsrc.rc oledlg_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add version.rc shlwapi_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add rsrc.rc wininet_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add winmm_res.rc winmm_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add wldap32.rc wldap32_En.rc</t>
+  </si>
+  <si>
+    <t>call :lang_add localui.rc ui_En.rc</t>
   </si>
 </sst>
 </file>
@@ -5810,7 +6018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E80C488-7D20-4452-BB4F-AFBA46CEFBDA}">
   <dimension ref="A1:J287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+    <sheetView topLeftCell="A173" workbookViewId="0">
       <selection activeCell="A180" sqref="A180"/>
     </sheetView>
   </sheetViews>
@@ -14628,4 +14836,535 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C7971E-918F-4E1A-B699-313CC3EFBFB7}">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>931</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>933</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>975</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>977</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>978</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>979</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>980</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>981</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>982</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>985</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>986</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>989</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>992</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1166</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>994</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1415</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>995</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>997</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>998</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1176</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1431</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>